<commit_message>
possible datasets found on Kaggle
</commit_message>
<xml_diff>
--- a/schedule/FinalProject_Team_1_Schedule.xlsx
+++ b/schedule/FinalProject_Team_1_Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\DSDegree\PennState\DAAN_881\FinalProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\btb51\Documents\GitHub\DAAN881_Team1\schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF01687B-DA18-4952-8FF8-4E9195CEEF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997A4913-1001-4899-93DE-F559D2773B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44895" yWindow="1785" windowWidth="22305" windowHeight="15600" xr2:uid="{C7483658-7BF3-4B45-9234-97BA6C7871DB}"/>
   </bookViews>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,16 +357,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="12">
     <dxf>
       <font>
         <color theme="4" tint="0.79998168889431442"/>
@@ -533,36 +529,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="0.79998168889431442"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -894,7 +860,7 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,9 +870,9 @@
     <col min="3" max="3" width="45.85546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -925,7 +891,7 @@
       <c r="E1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="10" t="s">
@@ -948,7 +914,7 @@
       <c r="D2" s="4">
         <v>3</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -968,10 +934,10 @@
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>45422</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -985,7 +951,7 @@
       <c r="C4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1002,8 +968,8 @@
       <c r="D5" s="4">
         <v>5</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>19</v>
+      <c r="H5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1019,7 +985,7 @@
       <c r="D6" s="4">
         <v>3</v>
       </c>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1033,7 +999,7 @@
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1047,7 +1013,7 @@
       <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="19" t="s">
+      <c r="H8" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1064,17 +1030,17 @@
       <c r="D9" s="4">
         <v>2</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1088,7 +1054,7 @@
       <c r="C12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1102,7 +1068,7 @@
       <c r="C13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1116,7 +1082,7 @@
       <c r="C14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="19" t="s">
+      <c r="H14" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1130,7 +1096,7 @@
       <c r="C15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1144,7 +1110,7 @@
       <c r="C16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1158,7 +1124,7 @@
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>